<commit_message>
added EF Core documentation
</commit_message>
<xml_diff>
--- a/src/EntityFramework/CRUDExample/wwwroot/templates/countries_template.xlsx
+++ b/src/EntityFramework/CRUDExample/wwwroot/templates/countries_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\ASPNETCore7\ASPNETCore7\src\EntityFramework\CRUDExample\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA79E3CC-E0FE-4322-A088-664D890C448D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0222383E-66D1-41EA-A590-6782B1A3BFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2625" windowWidth="21600" windowHeight="11295" xr2:uid="{B1F2AF36-6242-43EB-8347-2E7070823BB4}"/>
+    <workbookView xWindow="5145" yWindow="2970" windowWidth="21600" windowHeight="11295" xr2:uid="{B1F2AF36-6242-43EB-8347-2E7070823BB4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Countries" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>